<commit_message>
Update test form (text field instead of int)
</commit_message>
<xml_diff>
--- a/extras/test form/Example launch SMS.xlsx
+++ b/extras/test form/Example launch SMS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cking/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cking/github/surveycto-field-plug-ins/example-launch-sms/extras/test form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CF7FD7-39EE-D044-97C4-F3808C4FB5D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0B7A08-0BE1-C14B-A56C-48306D12AD2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="386">
   <si>
     <t>type</t>
   </si>
@@ -2638,6 +2638,9 @@
   </si>
   <si>
     <t>example_launch_sms</t>
+  </si>
+  <si>
+    <t>numbers_phone</t>
   </si>
 </sst>
 </file>
@@ -3346,7 +3349,206 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="160">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4789,9 +4991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5044,13 +5246,16 @@
     </row>
     <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>374</v>
       </c>
       <c r="C11" t="s">
         <v>375</v>
+      </c>
+      <c r="F11" t="s">
+        <v>385</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>358</v>
@@ -5102,139 +5307,233 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B1:C1048576 I1:I1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576 I1:I1048576 F1:F10 F12:F1048576">
+    <cfRule type="expression" dxfId="159" priority="75" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 O1:O1048576 I1:I1048576">
-    <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="72" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="131" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576 F1:F10 F12:F1048576">
+    <cfRule type="expression" dxfId="157" priority="69" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="130" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="67" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="129" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="65" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576 F1:F10 F12:F1048576">
+    <cfRule type="expression" dxfId="154" priority="60" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="127" priority="24" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F10 B1:B1048576 F12:F1048576">
+    <cfRule type="expression" dxfId="153" priority="50" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="44" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="46" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="48" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="123" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="42" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="122" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576 F1:F10 F12:F1048576">
+    <cfRule type="expression" dxfId="148" priority="40" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C1048576 F1:F10 F12:F1048576">
+    <cfRule type="expression" dxfId="147" priority="36" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="120" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="34" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="119" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:W10 A12:W1048576 A11:E11 G11:W11">
+    <cfRule type="expression" dxfId="145" priority="28" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="31" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="35" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="37" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="41" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="43" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="45" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="47" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="49" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="51" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="54" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="61" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="66" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="68" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="70" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="71" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="73" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="74" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="76" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="29" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B1048576 F1:F10 F12:F1048576">
+    <cfRule type="expression" dxfId="125" priority="27" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
+      <formula>$A11="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="24" priority="20" stopIfTrue="1">
+      <formula>$A11="text"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A11, 16)="select_multiple ", LEN($A11)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A11, 17)))), AND(LEFT($A11, 11)="select_one ", LEN($A11)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A11, 12)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="22" priority="13" stopIfTrue="1">
+      <formula>OR($A11="audio audit", $A11="text audit", $A11="speed violations count", $A11="speed violations list", $A11="speed violations audit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
+      <formula>OR($A11="date", $A11="datetime")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
+      <formula>$A11="image"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A11, 14)="sensor_stream ", LEN($A11)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A11, 15)))), AND(LEFT($A11, 17)="sensor_statistic ", LEN($A11)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A11, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="3" stopIfTrue="1">
+      <formula>$A11="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="4" stopIfTrue="1">
+      <formula>OR($A11="audio", $A11="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
+      <formula>$A11="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="8" stopIfTrue="1">
+      <formula>OR($A11="date", $A11="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
+      <formula>OR($A11="calculate", $A11="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="10" stopIfTrue="1">
+      <formula>$A11="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
+      <formula>$A11="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+      <formula>OR($A11="geopoint", $A11="geoshape", $A11="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14" stopIfTrue="1">
+      <formula>OR($A11="audio audit", $A11="text audit", $A11="speed violations count", $A11="speed violations list", $A11="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15" stopIfTrue="1">
+      <formula>OR($A11="username", $A11="phonenumber", $A11="start", $A11="end", $A11="deviceid", $A11="subscriberid", $A11="simserial", $A11="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="17" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A11, 16)="select_multiple ", LEN($A11)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A11, 17)))), AND(LEFT($A11, 11)="select_one ", LEN($A11)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A11, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="18" stopIfTrue="1">
+      <formula>$A11="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="19" stopIfTrue="1">
+      <formula>$A11="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="21" stopIfTrue="1">
+      <formula>$A11="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="22" stopIfTrue="1">
+      <formula>$A11="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="23" stopIfTrue="1">
+      <formula>$A11="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="24" stopIfTrue="1">
+      <formula>$A11="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="26" stopIfTrue="1">
+      <formula>$A11="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A11, 14)="sensor_stream ", LEN($A11)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A11, 15)))), AND(LEFT($A11, 17)="sensor_statistic ", LEN($A11)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A11, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5340,7 +5639,7 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:H2000">
-    <cfRule type="expression" dxfId="98" priority="1">
+    <cfRule type="expression" dxfId="124" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5354,7 +5653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5398,7 +5697,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003051401</v>
+        <v>2003061123</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>
@@ -9234,348 +9533,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>